<commit_message>
Added first three rows with commands and icons.
</commit_message>
<xml_diff>
--- a/command_lookup.xlsx
+++ b/command_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Android\AndroidRemoteHotkey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFF6827-5392-4ACB-814A-25E217D9BABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6532A699-D8AC-49E7-AD14-430D01022F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-63960" yWindow="90" windowWidth="12705" windowHeight="21420" xr2:uid="{6CD02E4E-62D4-41A8-B384-15CB0D8E790B}"/>
+    <workbookView xWindow="-51120" yWindow="240" windowWidth="12480" windowHeight="21120" xr2:uid="{6CD02E4E-62D4-41A8-B384-15CB0D8E790B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
   <si>
     <t>CTRL</t>
   </si>
@@ -208,9 +208,6 @@
     <t>TeamViewer</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>VMWare</t>
   </si>
   <si>
@@ -332,6 +329,36 @@
   </si>
   <si>
     <t>subl</t>
+  </si>
+  <si>
+    <t>jlink</t>
+  </si>
+  <si>
+    <t>flutter</t>
+  </si>
+  <si>
+    <t>w11</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>linux</t>
+  </si>
+  <si>
+    <t>teamv</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>NUM0</t>
+  </si>
+  <si>
+    <t>0x18</t>
+  </si>
+  <si>
+    <t>0x62</t>
   </si>
 </sst>
 </file>
@@ -725,7 +752,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1073,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -1063,10 +1090,10 @@
         <v>C2</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1077,7 +1104,7 @@
         <v>43</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
@@ -1094,10 +1121,10 @@
         <v>A2</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1108,7 +1135,7 @@
         <v>42</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
@@ -1125,10 +1152,10 @@
         <v>A2</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1139,7 +1166,7 @@
         <v>41</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="6">
         <v>1</v>
@@ -1156,10 +1183,10 @@
         <v>C2</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1170,7 +1197,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="6">
         <v>1</v>
@@ -1187,7 +1214,7 @@
         <v>A2</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>33</v>
@@ -1201,7 +1228,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
@@ -1218,7 +1245,7 @@
         <v>A2</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>32</v>
@@ -1232,7 +1259,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" s="6">
         <v>1</v>
@@ -1249,10 +1276,10 @@
         <v>A2</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1263,7 +1290,7 @@
         <v>47</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" s="3">
         <v>1</v>
@@ -1282,10 +1309,10 @@
         <v>A2</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1296,7 +1323,7 @@
         <v>48</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
@@ -1313,10 +1340,10 @@
         <v>A2</v>
       </c>
       <c r="J18" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K18" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1327,7 +1354,7 @@
         <v>50</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
@@ -1347,10 +1374,10 @@
         <v>E2</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1360,6 +1387,9 @@
       <c r="B20" s="6" t="s">
         <v>51</v>
       </c>
+      <c r="C20" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="D20" s="6">
         <v>1</v>
       </c>
@@ -1375,10 +1405,10 @@
         <v>C2</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1388,6 +1418,9 @@
       <c r="B21" s="6" t="s">
         <v>52</v>
       </c>
+      <c r="C21" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="D21" s="6">
         <v>1</v>
       </c>
@@ -1403,10 +1436,10 @@
         <v>A2</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1416,6 +1449,9 @@
       <c r="B22" s="6" t="s">
         <v>53</v>
       </c>
+      <c r="C22" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="D22" s="6">
         <v>1</v>
       </c>
@@ -1434,10 +1470,10 @@
         <v>E2</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1447,6 +1483,9 @@
       <c r="B23" s="6" t="s">
         <v>54</v>
       </c>
+      <c r="C23" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="D23" s="6">
         <v>1</v>
       </c>
@@ -1468,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1478,6 +1517,9 @@
       <c r="B24" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="C24" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="D24" s="6">
         <v>1</v>
       </c>
@@ -1496,10 +1538,10 @@
         <v>E2</v>
       </c>
       <c r="J24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1509,7 +1551,9 @@
       <c r="B25" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="D25" s="3">
         <v>1</v>
       </c>
@@ -1527,21 +1571,19 @@
         <v>A2</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="B26" s="6"/>
       <c r="H26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H26:H45" si="2">D26*128+E26*64+F26*32+G26*16+2</f>
         <v>2</v>
       </c>
       <c r="I26" s="2" t="str">
@@ -1554,7 +1596,7 @@
         <v>26</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I27" s="2" t="str">
@@ -1567,7 +1609,7 @@
         <v>27</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I28" s="2" t="str">
@@ -1580,7 +1622,7 @@
         <v>28</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I29" s="2" t="str">
@@ -1593,7 +1635,7 @@
         <v>29</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I30" s="2" t="str">
@@ -1606,7 +1648,7 @@
         <v>30</v>
       </c>
       <c r="H31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I31" s="2" t="str">
@@ -1619,7 +1661,7 @@
         <v>31</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I32" s="2" t="str">
@@ -1638,7 +1680,7 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I33" s="5" t="str">
@@ -1653,15 +1695,30 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>226</v>
       </c>
       <c r="I34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>E2</v>
+      </c>
+      <c r="J34" t="s">
+        <v>72</v>
+      </c>
+      <c r="K34" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1669,67 +1726,148 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>226</v>
       </c>
       <c r="I35" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>E2</v>
+      </c>
+      <c r="J35" t="s">
+        <v>70</v>
+      </c>
+      <c r="K35" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
       <c r="H36" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>82</v>
       </c>
       <c r="I36" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>52</v>
+      </c>
+      <c r="J36" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
       <c r="H37" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>146</v>
       </c>
       <c r="I37" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>92</v>
+      </c>
+      <c r="J37" t="s">
+        <v>89</v>
+      </c>
+      <c r="K37" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
       <c r="H38" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>226</v>
       </c>
       <c r="I38" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>E2</v>
+      </c>
+      <c r="J38" t="s">
+        <v>69</v>
+      </c>
+      <c r="K38" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
       <c r="H39" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>226</v>
       </c>
       <c r="I39" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>E2</v>
+      </c>
+      <c r="J39" t="s">
+        <v>71</v>
+      </c>
+      <c r="K39" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -1737,15 +1875,27 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>64</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>162</v>
       </c>
       <c r="I40" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>A2</v>
+      </c>
+      <c r="J40" t="s">
+        <v>104</v>
+      </c>
+      <c r="K40" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1753,35 +1903,40 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3">
+        <v>1</v>
+      </c>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
       <c r="G41" s="3"/>
       <c r="H41" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>162</v>
       </c>
       <c r="I41" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
+        <v>A2</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
-        <v>63</v>
-      </c>
       <c r="H42" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I42" s="2" t="str">
@@ -1793,11 +1948,8 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
-        <v>64</v>
-      </c>
       <c r="H43" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I43" s="2" t="str">
@@ -1809,11 +1961,8 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
-        <v>65</v>
-      </c>
       <c r="H44" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I44" s="2" t="str">
@@ -1825,11 +1974,8 @@
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
-        <v>66</v>
-      </c>
       <c r="H45" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I45" s="2" t="str">

</xml_diff>

<commit_message>
Fixed permissions issue. Added TODOs
</commit_message>
<xml_diff>
--- a/command_lookup.xlsx
+++ b/command_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Android\AndroidRemoteHotkey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6532A699-D8AC-49E7-AD14-430D01022F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724AA6CB-72A1-45D8-A2A5-613963A91C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51120" yWindow="240" windowWidth="12480" windowHeight="21120" xr2:uid="{6CD02E4E-62D4-41A8-B384-15CB0D8E790B}"/>
+    <workbookView xWindow="-76920" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{6CD02E4E-62D4-41A8-B384-15CB0D8E790B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="109">
   <si>
     <t>CTRL</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t>0x62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;&gt; Need lookup table. </t>
   </si>
 </sst>
 </file>
@@ -749,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1713F471-F2EC-4DFB-9501-B5302C83F252}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +765,7 @@
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -797,7 +800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -833,8 +836,11 @@
       <c r="K2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -871,7 +877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -894,11 +900,11 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H49" si="0">D4*128+E4*64+F4*32+G4*16+2</f>
+        <f t="shared" ref="H4:H41" si="0">D4*128+E4*64+F4*32+G4*16+2</f>
         <v>162</v>
       </c>
       <c r="I4" s="2" t="str">
-        <f t="shared" ref="I4:I49" si="1">DEC2HEX(H4)</f>
+        <f t="shared" ref="I4:I41" si="1">DEC2HEX(H4)</f>
         <v>A2</v>
       </c>
       <c r="J4" t="s">
@@ -908,7 +914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -939,7 +945,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -970,7 +976,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1096,7 +1102,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1127,7 +1133,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1158,7 +1164,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1189,7 +1195,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1220,7 +1226,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1251,7 +1257,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1581,456 +1587,344 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
       <c r="H26" s="1">
-        <f t="shared" ref="H26:H45" si="2">D26*128+E26*64+F26*32+G26*16+2</f>
-        <v>2</v>
+        <f t="shared" ref="H26:H37" si="2">D26*128+E26*64+F26*32+G26*16+2</f>
+        <v>226</v>
       </c>
       <c r="I26" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>E2</v>
+      </c>
+      <c r="J26" t="s">
+        <v>72</v>
+      </c>
+      <c r="K26" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
       <c r="H27" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>226</v>
       </c>
       <c r="I27" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>E2</v>
+      </c>
+      <c r="J27" t="s">
+        <v>70</v>
+      </c>
+      <c r="K27" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
       <c r="H28" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>82</v>
       </c>
       <c r="I28" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>52</v>
+      </c>
+      <c r="J28" t="s">
+        <v>68</v>
+      </c>
+      <c r="K28" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
       <c r="H29" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>146</v>
       </c>
       <c r="I29" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>92</v>
+      </c>
+      <c r="J29" t="s">
+        <v>89</v>
+      </c>
+      <c r="K29" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
       <c r="H30" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>226</v>
       </c>
       <c r="I30" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>E2</v>
+      </c>
+      <c r="J30" t="s">
+        <v>69</v>
+      </c>
+      <c r="K30" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
       <c r="H31" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>226</v>
       </c>
       <c r="I31" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>E2</v>
+      </c>
+      <c r="J31" t="s">
+        <v>71</v>
+      </c>
+      <c r="K31" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
       <c r="H32" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>162</v>
       </c>
       <c r="I32" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>A2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>104</v>
+      </c>
+      <c r="K32" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B33" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
       <c r="G33" s="3"/>
       <c r="H33" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>162</v>
       </c>
       <c r="I33" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
+        <v>A2</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
       <c r="H34" s="1">
         <f t="shared" si="2"/>
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="I34" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>E2</v>
-      </c>
-      <c r="J34" t="s">
-        <v>72</v>
-      </c>
-      <c r="K34" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
       <c r="H35" s="1">
         <f t="shared" si="2"/>
-        <v>226</v>
+        <v>2</v>
       </c>
       <c r="I35" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>E2</v>
-      </c>
-      <c r="J35" t="s">
-        <v>70</v>
-      </c>
-      <c r="K35" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
       <c r="H36" s="1">
         <f t="shared" si="2"/>
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="I36" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>52</v>
-      </c>
-      <c r="J36" t="s">
-        <v>68</v>
-      </c>
-      <c r="K36" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
       <c r="H37" s="1">
         <f t="shared" si="2"/>
-        <v>146</v>
+        <v>2</v>
       </c>
       <c r="I37" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>92</v>
-      </c>
-      <c r="J37" t="s">
-        <v>89</v>
-      </c>
-      <c r="K37" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
       <c r="H38" s="1">
-        <f t="shared" si="2"/>
-        <v>226</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="I38" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>E2</v>
-      </c>
-      <c r="J38" t="s">
-        <v>69</v>
-      </c>
-      <c r="K38" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
       <c r="H39" s="1">
-        <f t="shared" si="2"/>
-        <v>226</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="I39" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>E2</v>
-      </c>
-      <c r="J39" t="s">
-        <v>71</v>
-      </c>
-      <c r="K39" t="s">
-        <v>76</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
       <c r="H40" s="1">
-        <f t="shared" si="2"/>
-        <v>162</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="I40" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>A2</v>
-      </c>
-      <c r="J40" t="s">
-        <v>104</v>
-      </c>
-      <c r="K40" t="s">
-        <v>106</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" s="3">
-        <v>1</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3">
-        <v>1</v>
-      </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="4">
-        <f t="shared" si="2"/>
-        <v>162</v>
-      </c>
-      <c r="I41" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>A2</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="H42" s="1">
-        <f t="shared" si="2"/>
+      <c r="H41" s="1">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I42" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="H43" s="1">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I43" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="H44" s="1">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I44" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="H45" s="1">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="I45" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="H46" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I46" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="H47" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I47" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="H48" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I48" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="H49" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I49" s="2" t="str">
+      <c r="I41" s="2" t="str">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Updated commands for Windows VirtualKeys, added Toast. Added Row 4.
</commit_message>
<xml_diff>
--- a/command_lookup.xlsx
+++ b/command_lookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Android\AndroidRemoteHotkey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724AA6CB-72A1-45D8-A2A5-613963A91C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BC517D-4BCE-450E-8AAD-813A0724C3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-76920" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{6CD02E4E-62D4-41A8-B384-15CB0D8E790B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="116">
   <si>
     <t>CTRL</t>
   </si>
@@ -208,33 +208,9 @@
     <t>TeamViewer</t>
   </si>
   <si>
-    <t>VMWare</t>
-  </si>
-  <si>
     <t>Pushbullet</t>
   </si>
   <si>
-    <t>FancyZones</t>
-  </si>
-  <si>
-    <t>PinWindow</t>
-  </si>
-  <si>
-    <t>&lt;pin clipart&gt;</t>
-  </si>
-  <si>
-    <t>Command Prompt</t>
-  </si>
-  <si>
-    <t>Chrome Regular</t>
-  </si>
-  <si>
-    <t>Ungoogled Chrome</t>
-  </si>
-  <si>
-    <t>Signal Messenger</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -307,12 +283,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>MINUS</t>
-  </si>
-  <si>
-    <t>EQUALS</t>
-  </si>
-  <si>
     <t>0x1E</t>
   </si>
   <si>
@@ -325,9 +295,6 @@
     <t>0x17</t>
   </si>
   <si>
-    <t>0x2E</t>
-  </si>
-  <si>
     <t>subl</t>
   </si>
   <si>
@@ -361,14 +328,68 @@
     <t>0x62</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;&gt; Need lookup table. </t>
+    <t>newByte(For Windows)</t>
+  </si>
+  <si>
+    <t>AsHex</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>vmware</t>
+  </si>
+  <si>
+    <t>pushbullet</t>
+  </si>
+  <si>
+    <t>powertoys</t>
+  </si>
+  <si>
+    <t>pushpin</t>
+  </si>
+  <si>
+    <t>cmd</t>
+  </si>
+  <si>
+    <t>gchrome</t>
+  </si>
+  <si>
+    <t>chromium</t>
+  </si>
+  <si>
+    <t>signal</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>Pin Window</t>
+  </si>
+  <si>
+    <t>Tiling Zones</t>
+  </si>
+  <si>
+    <t>VMware</t>
+  </si>
+  <si>
+    <t>Ungoogled</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>TODO:.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,13 +405,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -420,10 +465,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -438,8 +485,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -752,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1713F471-F2EC-4DFB-9501-B5302C83F252}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +824,7 @@
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -799,8 +858,17 @@
       <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -833,14 +901,19 @@
       <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>57</v>
+      </c>
+      <c r="M2" s="2" t="str">
+        <f>DEC2HEX(L2)</f>
+        <v>39</v>
+      </c>
+      <c r="N2" s="15"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -873,11 +946,19 @@
       <c r="J3" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>48</v>
+      </c>
+      <c r="M3" s="2" t="str">
+        <f t="shared" ref="M3:M33" si="0">DEC2HEX(L3)</f>
+        <v>30</v>
+      </c>
+      <c r="N3" s="15"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -900,21 +981,29 @@
         <v>0</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H41" si="0">D4*128+E4*64+F4*32+G4*16+2</f>
+        <f t="shared" ref="H4:H41" si="1">D4*128+E4*64+F4*32+G4*16+2</f>
         <v>162</v>
       </c>
       <c r="I4" s="2" t="str">
-        <f t="shared" ref="I4:I41" si="1">DEC2HEX(H4)</f>
+        <f t="shared" ref="I4:I41" si="2">DEC2HEX(H4)</f>
         <v>A2</v>
       </c>
       <c r="J4" t="s">
         <v>14</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>83</v>
+      </c>
+      <c r="M4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="N4" s="15"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -931,21 +1020,29 @@
         <v>1</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="I5" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>68</v>
+      </c>
+      <c r="M5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="N5" s="15"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -962,21 +1059,29 @@
         <v>1</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>194</v>
       </c>
       <c r="I6" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C2</v>
       </c>
       <c r="J6" t="s">
         <v>19</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>80</v>
+      </c>
+      <c r="M6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="N6" s="15"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -993,21 +1098,29 @@
         <v>1</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>194</v>
       </c>
       <c r="I7" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C2</v>
       </c>
       <c r="J7" t="s">
         <v>21</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>67</v>
+      </c>
+      <c r="M7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="N7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1024,21 +1137,29 @@
         <v>1</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>194</v>
       </c>
       <c r="I8" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C2</v>
       </c>
       <c r="J8" t="s">
         <v>14</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>83</v>
+      </c>
+      <c r="M8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1057,21 +1178,29 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>194</v>
       </c>
       <c r="I9" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C2</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K9" s="13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>71</v>
+      </c>
+      <c r="M9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1079,7 +1208,7 @@
         <v>40</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -1088,21 +1217,29 @@
         <v>1</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>194</v>
       </c>
       <c r="I10" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C2</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10">
+        <v>65</v>
+      </c>
+      <c r="M10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1110,7 +1247,7 @@
         <v>43</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
@@ -1119,21 +1256,29 @@
         <v>1</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="I11" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="L11">
+        <v>65</v>
+      </c>
+      <c r="M11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="N11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1141,7 +1286,7 @@
         <v>42</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
@@ -1150,21 +1295,29 @@
         <v>1</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="I12" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12">
+        <v>69</v>
+      </c>
+      <c r="M12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="N12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1172,7 +1325,7 @@
         <v>41</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D13" s="6">
         <v>1</v>
@@ -1181,21 +1334,29 @@
         <v>1</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>194</v>
       </c>
       <c r="I13" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C2</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13">
+        <v>70</v>
+      </c>
+      <c r="M13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="N13" s="15"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1203,7 +1364,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D14" s="6">
         <v>1</v>
@@ -1212,21 +1373,29 @@
         <v>1</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="I14" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" s="14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>67</v>
+      </c>
+      <c r="M14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1234,7 +1403,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
@@ -1243,21 +1412,29 @@
         <v>1</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="I15" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="K15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>80</v>
+      </c>
+      <c r="M15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1265,7 +1442,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D16" s="6">
         <v>1</v>
@@ -1274,21 +1451,29 @@
         <v>1</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="I16" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16">
+        <v>77</v>
+      </c>
+      <c r="M16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4D</v>
+      </c>
+      <c r="N16" s="15"/>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1296,7 +1481,7 @@
         <v>47</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D17" s="3">
         <v>1</v>
@@ -1307,21 +1492,29 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="I17" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17">
+        <v>86</v>
+      </c>
+      <c r="M17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1329,7 +1522,7 @@
         <v>48</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
@@ -1338,21 +1531,29 @@
         <v>1</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="I18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="L18">
+        <v>107</v>
+      </c>
+      <c r="M18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>6B</v>
+      </c>
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1360,33 +1561,41 @@
         <v>50</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="1"/>
+        <v>226</v>
+      </c>
+      <c r="I19" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>E2</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19">
         <v>78</v>
       </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" s="6">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1">
-        <f t="shared" si="0"/>
-        <v>226</v>
-      </c>
-      <c r="I19" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>E2</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4E</v>
+      </c>
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1394,7 +1603,7 @@
         <v>51</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D20" s="6">
         <v>1</v>
@@ -1403,21 +1612,29 @@
         <v>1</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>194</v>
       </c>
       <c r="I20" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>C2</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="K20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20">
+        <v>86</v>
+      </c>
+      <c r="M20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1425,7 +1642,7 @@
         <v>52</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
@@ -1434,21 +1651,29 @@
         <v>1</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="I21" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="K21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="K21" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21">
+        <v>70</v>
+      </c>
+      <c r="M21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1456,7 +1681,7 @@
         <v>53</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D22" s="6">
         <v>1</v>
@@ -1468,21 +1693,29 @@
         <v>1</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>226</v>
       </c>
       <c r="I22" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E2</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="K22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="10">
+        <v>2</v>
+      </c>
+      <c r="K22" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="L22">
+        <v>50</v>
+      </c>
+      <c r="M22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1490,7 +1723,7 @@
         <v>54</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D23" s="6">
         <v>1</v>
@@ -1502,21 +1735,29 @@
         <v>1</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>226</v>
       </c>
       <c r="I23" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E2</v>
       </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="K23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="11">
+        <v>1</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="L23">
+        <v>49</v>
+      </c>
+      <c r="M23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1524,7 +1765,7 @@
         <v>55</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D24" s="6">
         <v>1</v>
@@ -1536,21 +1777,27 @@
         <v>1</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>226</v>
       </c>
       <c r="I24" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E2</v>
       </c>
       <c r="J24" t="s">
-        <v>91</v>
-      </c>
-      <c r="K24" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="K24" s="12"/>
+      <c r="L24">
+        <v>76</v>
+      </c>
+      <c r="M24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4C</v>
+      </c>
+      <c r="N24" s="15"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1558,7 +1805,7 @@
         <v>56</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
@@ -1569,26 +1816,37 @@
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
       <c r="I25" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="L25">
+        <v>84</v>
+      </c>
+      <c r="M25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="N25" s="15"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>112</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1600,26 +1858,37 @@
         <v>1</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" ref="H26:H37" si="2">D26*128+E26*64+F26*32+G26*16+2</f>
+        <f t="shared" ref="H26:H37" si="3">D26*128+E26*64+F26*32+G26*16+2</f>
         <v>226</v>
       </c>
       <c r="I26" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E2</v>
       </c>
       <c r="J26" t="s">
-        <v>72</v>
-      </c>
-      <c r="K26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="L26">
+        <v>86</v>
+      </c>
+      <c r="M26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="N26" s="15"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1631,26 +1900,37 @@
         <v>1</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>226</v>
       </c>
       <c r="I27" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E2</v>
       </c>
       <c r="J27" t="s">
-        <v>70</v>
-      </c>
-      <c r="K27" t="s">
+        <v>62</v>
+      </c>
+      <c r="K27" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>80</v>
+      </c>
+      <c r="M27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="N27" s="15"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>111</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1659,29 +1939,37 @@
         <v>1</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
       <c r="I28" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="J28" t="s">
-        <v>68</v>
-      </c>
-      <c r="K28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L28">
+        <v>70</v>
+      </c>
+      <c r="M28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="N28" s="15"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1690,26 +1978,37 @@
         <v>1</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>146</v>
       </c>
       <c r="I29" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92</v>
       </c>
       <c r="J29" t="s">
-        <v>89</v>
-      </c>
-      <c r="K29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="L29">
+        <v>84</v>
+      </c>
+      <c r="M29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="N29" s="15"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>105</v>
+      </c>
+      <c r="C30" t="s">
+        <v>105</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1721,57 +2020,79 @@
         <v>1</v>
       </c>
       <c r="H30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>226</v>
       </c>
       <c r="I30" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>E2</v>
       </c>
       <c r="J30" t="s">
-        <v>69</v>
-      </c>
-      <c r="K30" t="s">
+        <v>61</v>
+      </c>
+      <c r="K30" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>67</v>
+      </c>
+      <c r="M30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="N30" s="15"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="3"/>
+        <v>226</v>
+      </c>
+      <c r="I31" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>E2</v>
+      </c>
+      <c r="J31" t="s">
         <v>63</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="H31" s="1">
-        <f t="shared" si="2"/>
-        <v>226</v>
-      </c>
-      <c r="I31" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>E2</v>
-      </c>
-      <c r="J31" t="s">
-        <v>71</v>
-      </c>
-      <c r="K31" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L31">
+        <v>77</v>
+      </c>
+      <c r="M31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4D</v>
+      </c>
+      <c r="N31" s="15"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>113</v>
+      </c>
+      <c r="C32" t="s">
+        <v>107</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1780,28 +2101,38 @@
         <v>1</v>
       </c>
       <c r="H32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>162</v>
       </c>
       <c r="I32" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J32" t="s">
-        <v>104</v>
-      </c>
-      <c r="K32" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="L32">
+        <v>85</v>
+      </c>
+      <c r="M32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="N32" s="15"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="D33" s="3">
         <v>1</v>
       </c>
@@ -1811,121 +2142,132 @@
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>162</v>
       </c>
       <c r="I33" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>A2</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="L33">
+        <v>96</v>
+      </c>
+      <c r="M33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="N33" s="15"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
+      <c r="B34" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="H34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I34" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I35" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="H36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I36" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="H37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I37" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I38" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="H39" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I39" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="H40" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I40" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="H41" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I41" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added screenshot, minor modifications.
</commit_message>
<xml_diff>
--- a/command_lookup.xlsx
+++ b/command_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Android\AndroidRemoteHotkey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E4236A-A07C-4B6C-890F-D6EE69AFBFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66569C26-2AA2-4A13-A078-158D426BB215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="3285" windowWidth="28800" windowHeight="15555" xr2:uid="{6CD02E4E-62D4-41A8-B384-15CB0D8E790B}"/>
+    <workbookView xWindow="-20550" yWindow="5040" windowWidth="16200" windowHeight="28485" xr2:uid="{6CD02E4E-62D4-41A8-B384-15CB0D8E790B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="110">
   <si>
     <t>CTRL</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>Esc</t>
+  </si>
+  <si>
+    <t>VS Code</t>
+  </si>
+  <si>
+    <t>vscodium</t>
   </si>
 </sst>
 </file>
@@ -791,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1713F471-F2EC-4DFB-9501-B5302C83F252}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +922,7 @@
         <v>48</v>
       </c>
       <c r="L3" s="2" t="str">
-        <f t="shared" ref="L3:L42" si="0">DEC2HEX(K3)</f>
+        <f t="shared" ref="L3:L43" si="0">DEC2HEX(K3)</f>
         <v>30</v>
       </c>
     </row>
@@ -2326,15 +2332,40 @@
       <c r="A43" s="3">
         <v>40</v>
       </c>
-      <c r="H43" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="I43" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J43" s="11"/>
+      <c r="B43" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="4">
+        <f t="shared" si="1"/>
+        <v>226</v>
+      </c>
+      <c r="I43" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>E2</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K43">
+        <v>86</v>
+      </c>
+      <c r="L43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="6">

</xml_diff>

<commit_message>
Added multiple modes, Sublime Text, and Altium
</commit_message>
<xml_diff>
--- a/command_lookup.xlsx
+++ b/command_lookup.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Android\AndroidRemoteHotkey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Android\AndroidRemoteHotkey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66569C26-2AA2-4A13-A078-158D426BB215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3DC74C-7561-4532-913A-63F696CD95BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20550" yWindow="5040" windowWidth="16200" windowHeight="28485" xr2:uid="{6CD02E4E-62D4-41A8-B384-15CB0D8E790B}"/>
+    <workbookView xWindow="28845" yWindow="-12720" windowWidth="16110" windowHeight="14460" activeTab="1" xr2:uid="{6CD02E4E-62D4-41A8-B384-15CB0D8E790B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Vkey Reference" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="145">
   <si>
     <t>CTRL</t>
   </si>
@@ -335,41 +337,146 @@
     <t>Sublime Merge</t>
   </si>
   <si>
-    <t>TEMP-Jobsearch</t>
+    <t>microsoft keyboard codes</t>
+  </si>
+  <si>
+    <t>1password</t>
+  </si>
+  <si>
+    <t>SPACE</t>
+  </si>
+  <si>
+    <t>1pass</t>
+  </si>
+  <si>
+    <t>MSI Afterburner</t>
+  </si>
+  <si>
+    <t>Esc</t>
+  </si>
+  <si>
+    <t>VSCode</t>
+  </si>
+  <si>
+    <t>vscode</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Rustdesk</t>
+  </si>
+  <si>
+    <t>rustdesk</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>OpenBCI</t>
+  </si>
+  <si>
+    <t>openbci</t>
+  </si>
+  <si>
+    <t>Close window</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Delete Line (Sublime)</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>xout</t>
+  </si>
+  <si>
+    <t>bckspc</t>
+  </si>
+  <si>
+    <t>Select Text</t>
+  </si>
+  <si>
+    <t>select line</t>
+  </si>
+  <si>
+    <t>As Int</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
   <si>
     <t>J</t>
   </si>
   <si>
-    <t>microsoft keyboard codes</t>
-  </si>
-  <si>
-    <t>1password</t>
-  </si>
-  <si>
-    <t>SPACE</t>
-  </si>
-  <si>
-    <t>1pass</t>
-  </si>
-  <si>
-    <t>MSI Afterburner</t>
-  </si>
-  <si>
-    <t>Esc</t>
-  </si>
-  <si>
-    <t>VS Code</t>
-  </si>
-  <si>
-    <t>vscodium</t>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Indent</t>
+  </si>
+  <si>
+    <t>Unindent</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>', "</t>
+  </si>
+  <si>
+    <t>right-indent</t>
+  </si>
+  <si>
+    <t>left-indent</t>
+  </si>
+  <si>
+    <t>Find/Replace</t>
+  </si>
+  <si>
+    <t>find_replace</t>
+  </si>
+  <si>
+    <t>Working?</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,8 +500,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +519,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,7 +560,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -478,6 +599,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -797,19 +928,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1713F471-F2EC-4DFB-9501-B5302C83F252}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="K26" sqref="A1:M51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -838,7 +969,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K1" t="s">
         <v>69</v>
@@ -850,7 +981,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -888,7 +1019,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -922,11 +1053,11 @@
         <v>48</v>
       </c>
       <c r="L3" s="2" t="str">
-        <f t="shared" ref="L3:L43" si="0">DEC2HEX(K3)</f>
+        <f t="shared" ref="L3:L51" si="0">DEC2HEX(K3)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -943,11 +1074,11 @@
         <v>1</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H43" si="1">D4*128+E4*64+F4*32+G4*16+2</f>
+        <f t="shared" ref="H4:H51" si="1">D4*128+E4*64+F4*32+G4*16+2</f>
         <v>162</v>
       </c>
       <c r="I4" s="2" t="str">
-        <f t="shared" ref="I4:I43" si="2">DEC2HEX(H4)</f>
+        <f t="shared" ref="I4:I51" si="2">DEC2HEX(H4)</f>
         <v>A2</v>
       </c>
       <c r="J4" s="11" t="s">
@@ -961,7 +1092,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -996,7 +1127,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1031,7 +1162,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1068,7 +1199,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>96</v>
       </c>
@@ -1100,7 +1231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1135,7 +1266,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>99</v>
       </c>
@@ -1167,7 +1298,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -1204,7 +1335,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1239,7 +1370,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1274,7 +1405,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1309,7 +1440,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1347,7 +1478,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1382,7 +1513,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1417,7 +1548,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -1452,7 +1583,7 @@
         <v>4D</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -1489,7 +1620,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1524,7 +1655,7 @@
         <v>6B</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1562,7 +1693,7 @@
         <v>4E</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>19</v>
       </c>
@@ -1597,7 +1728,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20</v>
       </c>
@@ -1632,7 +1763,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21</v>
       </c>
@@ -1670,7 +1801,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1708,7 +1839,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1746,7 +1877,7 @@
         <v>4C</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -1783,7 +1914,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1821,7 +1952,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1859,7 +1990,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1894,7 +2025,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1929,7 +2060,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1956,7 +2087,7 @@
         <v>C2</v>
       </c>
       <c r="J32" s="21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K32">
         <v>27</v>
@@ -1966,7 +2097,7 @@
         <v>1B</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2004,7 +2135,7 @@
         <v>4D</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2039,7 +2170,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>32</v>
       </c>
@@ -2076,7 +2207,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2111,7 +2242,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2149,7 +2280,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2184,7 +2315,7 @@
         <v>4E</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2220,15 +2351,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="D40" s="6">
         <v>1</v>
@@ -2248,26 +2379,26 @@
         <v>E2</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="K40">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L40" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>4A</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4F</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>38</v>
       </c>
       <c r="B41" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" t="s">
         <v>103</v>
       </c>
-      <c r="C41" t="s">
-        <v>105</v>
-      </c>
       <c r="D41" s="6">
         <v>1</v>
       </c>
@@ -2286,7 +2417,7 @@
         <v>E2</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K41">
         <v>32</v>
@@ -2296,12 +2427,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>39</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -2328,83 +2459,217 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>40</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C43" s="3" t="s">
+      <c r="B43" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D43" s="3">
-        <v>1</v>
-      </c>
-      <c r="E43" s="3">
-        <v>1</v>
-      </c>
-      <c r="F43" s="3">
-        <v>1</v>
-      </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="4">
-        <f t="shared" si="1"/>
-        <v>226</v>
-      </c>
-      <c r="I43" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>E2</v>
-      </c>
-      <c r="J43" s="12" t="s">
-        <v>48</v>
+      <c r="C43" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="I43" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="K43">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="L43" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="I44" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="K44">
+        <v>79</v>
+      </c>
+      <c r="L44" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4F</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H45" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I45" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K45">
+        <v>82</v>
+      </c>
+      <c r="L45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H46" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I46" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K46">
+        <v>82</v>
+      </c>
+      <c r="L46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H47" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I47" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K47">
+        <v>82</v>
+      </c>
+      <c r="L47" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
         <v>45</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H48" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I48" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <v>82</v>
+      </c>
+      <c r="L48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
         <v>46</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H49" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I49" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>82</v>
+      </c>
+      <c r="L49" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
         <v>47</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H50" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I50" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K50">
+        <v>82</v>
+      </c>
+      <c r="L50" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
         <v>48</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I51" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K51">
+        <v>82</v>
+      </c>
+      <c r="L51" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2414,4 +2679,2362 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B33B13D-F56B-486A-8519-EBED2E82994A}">
+  <dimension ref="A1:R68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.44140625" style="22" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <f t="shared" ref="H2:H49" si="0">D2*128+E2*64+F2*32+G2*16+2</f>
+        <v>130</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f>DEC2HEX(H2)</f>
+        <v>82</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2">
+        <v>87</v>
+      </c>
+      <c r="L2" s="2" t="str">
+        <f>DEC2HEX(K2)</f>
+        <v>57</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N2" s="23"/>
+      <c r="O2" s="11">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="2" t="str">
+        <f>DEC2HEX(P2)</f>
+        <v>30</v>
+      </c>
+      <c r="R2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" si="0"/>
+        <v>194</v>
+      </c>
+      <c r="I3" s="2" t="str">
+        <f>DEC2HEX(H3)</f>
+        <v>C2</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="K3">
+        <v>75</v>
+      </c>
+      <c r="L3" s="2" t="str">
+        <f t="shared" ref="L3:L49" si="1">DEC2HEX(K3)</f>
+        <v>4B</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N3" s="23"/>
+      <c r="O3" s="11">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="2" t="str">
+        <f t="shared" ref="Q3:Q48" si="2">DEC2HEX(P3)</f>
+        <v>31</v>
+      </c>
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f t="shared" ref="I4:I49" si="3">DEC2HEX(H4)</f>
+        <v>82</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4">
+        <v>76</v>
+      </c>
+      <c r="L4" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>4C</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="N4" s="23"/>
+      <c r="O4" s="11">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="I5" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="K5">
+        <v>221</v>
+      </c>
+      <c r="L5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DD</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N5" s="23"/>
+      <c r="O5" s="11">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>51</v>
+      </c>
+      <c r="Q5" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="R5" s="2"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="18">
+        <v>1</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="I6" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K6">
+        <v>219</v>
+      </c>
+      <c r="L6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>DB</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="N6" s="23"/>
+      <c r="O6" s="11">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>52</v>
+      </c>
+      <c r="Q6" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="I7" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="K7">
+        <v>72</v>
+      </c>
+      <c r="L7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="N7" s="23"/>
+      <c r="O7" s="11">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>53</v>
+      </c>
+      <c r="Q7" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I8" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J8" s="21"/>
+      <c r="L8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="11">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I9" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="L9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="11">
+        <v>7</v>
+      </c>
+      <c r="P9">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="L10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="11">
+        <v>8</v>
+      </c>
+      <c r="P10">
+        <v>56</v>
+      </c>
+      <c r="Q10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="6"/>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="L11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="11">
+        <v>9</v>
+      </c>
+      <c r="P11">
+        <v>57</v>
+      </c>
+      <c r="Q11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="R11" s="2"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="6"/>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="L12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="P12">
+        <v>65</v>
+      </c>
+      <c r="Q12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="6"/>
+      <c r="H13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I13" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J13" s="10"/>
+      <c r="L13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="P13">
+        <v>66</v>
+      </c>
+      <c r="Q13" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="R13" s="2"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="6"/>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I14" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="L14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="P14">
+        <v>67</v>
+      </c>
+      <c r="Q14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="6"/>
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I15" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J15" s="10"/>
+      <c r="L15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="P15">
+        <v>68</v>
+      </c>
+      <c r="Q15" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="6"/>
+      <c r="H16" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I16" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J16" s="10"/>
+      <c r="L16" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="P16">
+        <v>69</v>
+      </c>
+      <c r="Q16" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I17" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J17" s="12"/>
+      <c r="L17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P17">
+        <v>70</v>
+      </c>
+      <c r="Q17" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="L18" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="P18">
+        <v>71</v>
+      </c>
+      <c r="Q18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="H19" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I19" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="L19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="P19">
+        <v>72</v>
+      </c>
+      <c r="Q19" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="H20" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="L20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="P20">
+        <v>73</v>
+      </c>
+      <c r="Q20" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="R20" s="2"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="H21" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I21" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="L21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="P21">
+        <v>74</v>
+      </c>
+      <c r="Q21" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>4A</v>
+      </c>
+      <c r="R21" s="2"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="H22" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I22" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="L22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="P22">
+        <v>75</v>
+      </c>
+      <c r="Q22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>4B</v>
+      </c>
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="H23" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I23" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="L23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="P23">
+        <v>76</v>
+      </c>
+      <c r="Q23" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>4C</v>
+      </c>
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="H24" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I24" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J24" s="11"/>
+      <c r="L24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="P24">
+        <v>77</v>
+      </c>
+      <c r="Q24" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>4D</v>
+      </c>
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I25" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J25" s="12"/>
+      <c r="L25" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="P25">
+        <v>78</v>
+      </c>
+      <c r="Q25" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>4E</v>
+      </c>
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="H26" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I26" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J26" s="11"/>
+      <c r="L26" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="P26">
+        <v>79</v>
+      </c>
+      <c r="Q26" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>4F</v>
+      </c>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="H27" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I27" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J27" s="11"/>
+      <c r="L27" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="P27">
+        <v>80</v>
+      </c>
+      <c r="Q27" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="H28" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I28" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J28" s="11"/>
+      <c r="L28" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="P28">
+        <v>81</v>
+      </c>
+      <c r="Q28" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="R28" s="2"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I29" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J29" s="11"/>
+      <c r="L29" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="P29">
+        <v>82</v>
+      </c>
+      <c r="Q29" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="R29" s="2"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I30" s="20" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J30" s="21"/>
+      <c r="L30" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="P30">
+        <v>83</v>
+      </c>
+      <c r="Q30" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="R30" s="2"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I31" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J31" s="11"/>
+      <c r="L31" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="P31">
+        <v>84</v>
+      </c>
+      <c r="Q31" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="R31" s="2"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I32" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J32" s="11"/>
+      <c r="L32" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="P32">
+        <v>85</v>
+      </c>
+      <c r="Q32" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="R32" s="2"/>
+    </row>
+    <row r="33" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I33" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J33" s="12"/>
+      <c r="L33" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="P33">
+        <v>86</v>
+      </c>
+      <c r="Q33" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="R33" s="2"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="H34" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I34" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J34" s="11"/>
+      <c r="L34" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="2"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="P34">
+        <v>87</v>
+      </c>
+      <c r="Q34" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="R34" s="2"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="H35" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I35" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J35" s="11"/>
+      <c r="L35" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="P35">
+        <v>88</v>
+      </c>
+      <c r="Q35" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="R35" s="2"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="H36" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I36" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J36" s="11"/>
+      <c r="L36" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="P36">
+        <v>89</v>
+      </c>
+      <c r="Q36" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="R36" s="2"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="H37" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I37" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J37" s="11"/>
+      <c r="L37" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="2"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="P37">
+        <v>90</v>
+      </c>
+      <c r="Q37" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>5A</v>
+      </c>
+      <c r="R37" s="2"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="H38" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I38" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J38" s="11"/>
+      <c r="L38" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="P38">
+        <v>219</v>
+      </c>
+      <c r="Q38" s="2" t="str">
+        <f>DEC2HEX(P38)</f>
+        <v>DB</v>
+      </c>
+      <c r="R38" s="2"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="H39" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I39" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J39" s="11"/>
+      <c r="L39" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="P39">
+        <v>220</v>
+      </c>
+      <c r="Q39" s="2" t="str">
+        <f>DEC2HEX(P39)</f>
+        <v>DC</v>
+      </c>
+      <c r="R39" s="2"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="H40" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I40" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J40" s="11"/>
+      <c r="L40" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="P40">
+        <v>221</v>
+      </c>
+      <c r="Q40" s="2" t="str">
+        <f>DEC2HEX(P40)</f>
+        <v>DD</v>
+      </c>
+      <c r="R40" s="2"/>
+    </row>
+    <row r="41" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="3">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="H41" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I41" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J41" s="11"/>
+      <c r="L41" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="P41">
+        <v>222</v>
+      </c>
+      <c r="Q41" s="2" t="str">
+        <f>DEC2HEX(P41)</f>
+        <v>DE</v>
+      </c>
+      <c r="R41" s="2"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="H42" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I42" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J42" s="11"/>
+      <c r="L42" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="N42" s="23"/>
+      <c r="Q42" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R42" s="2"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="H43" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I43" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J43" s="11"/>
+      <c r="L43" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="23"/>
+      <c r="Q43" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R43" s="2"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="H44" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I44" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L44" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" s="23"/>
+      <c r="Q44" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R44" s="2"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="H45" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I45" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L45" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="2"/>
+      <c r="N45" s="23"/>
+      <c r="Q45" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R45" s="2"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="H46" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I46" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L46" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="2"/>
+      <c r="N46" s="23"/>
+      <c r="Q46" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R46" s="2"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="H47" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I47" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L47" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M47" s="2"/>
+      <c r="N47" s="23"/>
+      <c r="Q47" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R47" s="2"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="H48" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I48" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L48" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M48" s="2"/>
+      <c r="N48" s="23"/>
+      <c r="Q48" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R48" s="2"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="H49" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I49" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L49" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M49" s="2"/>
+      <c r="N49" s="23"/>
+      <c r="Q49" s="2" t="str">
+        <f>DEC2HEX(P49)</f>
+        <v>0</v>
+      </c>
+      <c r="R49" s="2"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q50" s="2" t="str">
+        <f t="shared" ref="Q50:Q68" si="4">DEC2HEX(P50)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q51" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q52" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q53" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q54" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q55" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q56" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q57" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q58" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q59" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q60" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q61" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q62" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q63" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q64" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q65" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q66" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q67" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q68" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J1" r:id="rId1" xr:uid="{8AB0C2AF-5794-4A4C-BDF4-182CA8351684}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1436162C-A636-4AC1-B1E9-15EA9A0035CF}">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>48</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f>DEC2HEX(B2)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f t="shared" ref="C3:C49" si="0">DEC2HEX(B3)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>51</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>53</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>54</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>55</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>57</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12">
+        <v>65</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13">
+        <v>66</v>
+      </c>
+      <c r="C13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <v>67</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15">
+        <v>68</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <v>69</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17">
+        <v>70</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18">
+        <v>71</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19">
+        <v>72</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20">
+        <v>73</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22">
+        <v>75</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4B</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23">
+        <v>76</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4C</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24">
+        <v>77</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4D</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25">
+        <v>78</v>
+      </c>
+      <c r="C25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4E</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26">
+        <v>79</v>
+      </c>
+      <c r="C26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4F</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27">
+        <v>80</v>
+      </c>
+      <c r="C27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28">
+        <v>81</v>
+      </c>
+      <c r="C28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29">
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30">
+        <v>83</v>
+      </c>
+      <c r="C30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31">
+        <v>84</v>
+      </c>
+      <c r="C31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32">
+        <v>85</v>
+      </c>
+      <c r="C32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33">
+        <v>86</v>
+      </c>
+      <c r="C33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34">
+        <v>87</v>
+      </c>
+      <c r="C34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35">
+        <v>88</v>
+      </c>
+      <c r="C35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36">
+        <v>89</v>
+      </c>
+      <c r="C36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37">
+        <v>90</v>
+      </c>
+      <c r="C37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>5A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C47" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>